<commit_message>
Data acquisition IoT Edge layer
Literature review papers
</commit_message>
<xml_diff>
--- a/LITERATURE REVIEW/Lit matrix current (Feb Week 1).xlsx
+++ b/LITERATURE REVIEW/Lit matrix current (Feb Week 1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Agrippina Mwangi\Documents\GitHub\Renewable_Energy_Integration\LITERATURE REVIEW\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://solisservices-my.sharepoint.com/personal/a_w_mwangi_uu_nl/Documents/Documents/GitHub/Renewable_Energy_Integration/LITERATURE REVIEW/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B0CE878-0D21-42D2-A464-33DC448C2EE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="13_ncr:1_{0B0CE878-0D21-42D2-A464-33DC448C2EE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4462F885-D979-4251-8DA7-C019D6EB14FD}"/>
   <bookViews>
-    <workbookView xWindow="2616" yWindow="2616" windowWidth="17280" windowHeight="8964" xr2:uid="{497C0ADB-D672-4D47-81E2-3B9010C22FDB}"/>
+    <workbookView xWindow="11520" yWindow="768" windowWidth="11280" windowHeight="8964" xr2:uid="{497C0ADB-D672-4D47-81E2-3B9010C22FDB}"/>
   </bookViews>
   <sheets>
     <sheet name="Month 1" sheetId="1" r:id="rId1"/>
@@ -33,8 +33,46 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={E64ED06D-69EA-4BB9-849F-A9D171D7AA56}</author>
+    <author>tc={91A9622D-DD67-49D7-A787-D8D93026EFF3}</author>
+  </authors>
+  <commentList>
+    <comment ref="D16" authorId="0" shapeId="0" xr:uid="{E64ED06D-69EA-4BB9-849F-A9D171D7AA56}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    The framework creates the general approaches to the context prediction
+Create and support automated decision-making approaches for reasoning context for energy consumption and user comfort
+The energy system is highly distributed and CAEMS manages large amounts of energy-related data that has to be able to react rapidly and smartly when conditions change and for this task we use smoothies and predictive techniques for data from sensors.</t>
+      </text>
+    </comment>
+    <comment ref="E16" authorId="1" shapeId="0" xr:uid="{91A9622D-DD67-49D7-A787-D8D93026EFF3}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Context aware management process:-
+- Sensor data acquisition
+- Feature extraction
+- Ontology model
+- Context prediction
+Reply:
+    Keeping a record of time points and the value of the disturbances complicates the forecasting process and can lead to erroneous results. Filtering or smoothing of context time series is the necessary preliminary prediction stage for obtaining trends
+- Averaging methods
+- Exponential smoothing methods
+- Kalman filter</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="92">
   <si>
     <t>Title/Author</t>
   </si>
@@ -284,12 +322,99 @@
   <si>
     <t>Cloud reliability is a measure of probability that a cloud delivers the services as intended.</t>
   </si>
+  <si>
+    <t>Data acquisition literature review</t>
+  </si>
+  <si>
+    <t>Cheng-Wen Wu</t>
+  </si>
+  <si>
+    <t>Can IoT make Semiconductor great again?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There is not much evidence that IoT will likely give a great boost to the semiconductor industry in the near future due to limitations in global economy and energy consumption.
+If IoT is going to give a boost to stagnant semiconductor industry, what will be the key factors of its success? </t>
+  </si>
+  <si>
+    <t>Propose the symbiotic system model (SSM) for developing IoT devices and systems.
+Propose symbiosis-based test (SBT) for device and system test.</t>
+  </si>
+  <si>
+    <t>A symbiotic relationship (SR) is a relationship of mutual dependence between two different systems where one system's input is from the other system's output (&amp; vice versa)
+The twin system (SS) comprises of the primary or functional system and the secondary or test system</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>The article seeks to trigger more research activities regarding establishing a sound IoT platform that allows heterogeneous integration of technologies and partners to migrate certain industries based on the notion of IoT</t>
+  </si>
+  <si>
+    <t>Kyselova A.G
+Verbitskyi I V
+Kyselov G.D</t>
+  </si>
+  <si>
+    <t>Context-aware framework for energy management system</t>
+  </si>
+  <si>
+    <t>Need to have visibility on the context from the level of sensor data to the higher level sitauation awareness (actuator level)
+Explore the challenges in microgrid energy control systems</t>
+  </si>
+  <si>
+    <t>Proposes a CAEMS that presents data management solutions.
+These solutions include sensor data acquisition and time series forecasting, ontology model and context prediction model for analytical query processing past and future context data</t>
+  </si>
+  <si>
+    <t>Energy systems: 
+* Renewable energy integration, multidirectional power flow, reduced peak load leveling and load demand, bidirectional flow of communication in the system, uninterrupted power supply, and improved quality of electricity.
+Context prediction - ability to predict the future context information in order to provide proactive service to the actions of all electrical facilities (loads and generators)</t>
+  </si>
+  <si>
+    <r>
+      <t>Did not provide a good background for the case scenario of their work. It would have been good to see actual use cases in the microgrids showing how the proposed model would be implemented. 
+(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>The work focused on data management making an assumption on its acquisition)</t>
+    </r>
+  </si>
+  <si>
+    <t>Interesting feature of ontological modeling and context based predictions (Very good approaches to consider for distributed IoT Edge layer evaluation)
+My interest lies in how the data is collected, shared and how the sensors behave when exposed to different environments (remote or otherwise).</t>
+  </si>
+  <si>
+    <t>A Mawire
+R.R.J. van den Heetkamp
+M McPherson
+E Zhandire</t>
+  </si>
+  <si>
+    <t>Data acquisition and control of a thermal energy storage and cooking system</t>
+  </si>
+  <si>
+    <t>Data acquisition for the thermal energy solar system (Data points: Temperature, fluid flow rate, and power input)
+Use of HP34970A data loggers (embedded with ADC)</t>
+  </si>
+  <si>
+    <t>The temperature contorl program is able to maintain a nearly constant charging temperature of the TES system.</t>
+  </si>
+  <si>
+    <t>Data acquisition system design and evaluation was done for thermal based small scale system</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -309,6 +434,12 @@
       <color theme="1"/>
       <name val="Century Gothic"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -331,13 +462,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -354,6 +488,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Mwangi, A.W. (Agrippina Wanjiru)" id="{B4096CF1-0946-4927-916B-75460E63E750}" userId="S::a.w.mwangi@uu.nl::46517c3c-63dd-4f94-8fd6-d3c21a943425" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -651,20 +791,48 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="D16" dT="2022-02-11T11:01:10.22" personId="{B4096CF1-0946-4927-916B-75460E63E750}" id="{E64ED06D-69EA-4BB9-849F-A9D171D7AA56}">
+    <text>The framework creates the general approaches to the context prediction
+Create and support automated decision-making approaches for reasoning context for energy consumption and user comfort
+The energy system is highly distributed and CAEMS manages large amounts of energy-related data that has to be able to react rapidly and smartly when conditions change and for this task we use smoothies and predictive techniques for data from sensors.</text>
+  </threadedComment>
+  <threadedComment ref="E16" dT="2022-02-11T11:03:49.59" personId="{B4096CF1-0946-4927-916B-75460E63E750}" id="{91A9622D-DD67-49D7-A787-D8D93026EFF3}">
+    <text>Context aware management process:-
+- Sensor data acquisition
+- Feature extraction
+- Ontology model
+- Context prediction</text>
+  </threadedComment>
+  <threadedComment ref="E16" dT="2022-02-11T11:09:15.58" personId="{B4096CF1-0946-4927-916B-75460E63E750}" id="{34D54E52-291F-40AE-823E-E9D6F3E6F044}" parentId="{91A9622D-DD67-49D7-A787-D8D93026EFF3}">
+    <text>Keeping a record of time points and the value of the disturbances complicates the forecasting process and can lead to erroneous results. Filtering or smoothing of context time series is the necessary preliminary prediction stage for obtaining trends
+- Averaging methods
+- Exponential smoothing methods
+- Kalman filter</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99C6CAC5-4A2C-4BDD-A220-11C3DA4654B6}">
-  <dimension ref="A1:H13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99C6CAC5-4A2C-4BDD-A220-11C3DA4654B6}">
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="5" width="22.44140625" style="1"/>
+    <col min="1" max="1" width="22.44140625" style="1"/>
+    <col min="2" max="2" width="24.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.21875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.77734375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="27.88671875" style="1" customWidth="1"/>
     <col min="6" max="6" width="26.21875" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="22.44140625" style="1"/>
+    <col min="7" max="7" width="27.109375" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="22.44140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
@@ -909,8 +1077,89 @@
         <v>71</v>
       </c>
     </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B14" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+    </row>
+    <row r="15" spans="1:8" ht="132" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="184.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="105.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B14:H14"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>